<commit_message>
socio dada 360 sizer
</commit_message>
<xml_diff>
--- a/data/country.xlsx
+++ b/data/country.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:AH28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,27 +441,167 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>CO2#Per#Population</t>
+          <t>0_0#Abs#0_0</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>GDP#Per#Population</t>
+          <t>95_99#Per#Population</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Happy#Ratio#Population</t>
+          <t>Alcohol_liter#Per#Adult</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Land#Abs#Land</t>
+          <t>Artists#Per#Population</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Baby#Per#Population</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Buddhist#Per#Population</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Cancer#Per#Population</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Centenary#Per#Population</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Christian#Per#Population</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Crimes#Per#Population</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Culture_budget#Per#Population</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Death#Per#Population</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Depression#Per#Population</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Divorce#Per#Population</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Doctor#Per#Population</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Drug_use#Per#Population</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Family_size#Per#Household</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Female#Per#Population</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Jewish#Per#Population</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Left_behind#Per#Population</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Life_expectancy#Age#Year</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Marriage#Per#Population</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Muslim#Per#Population</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Obesity#Per#Population</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
           <t>Population#Abs#Population</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Prisoners#Per#Population</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Retired#Per#Population</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Smoker#Per#Population</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Student#Per#Population</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Suicide#Per#Population</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>University#Per#Population</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Urban#Per#Population</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Vegetables#Per#Population</t>
         </is>
       </c>
     </row>
@@ -472,19 +612,101 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J2" t="n">
+        <v>3</v>
+      </c>
+      <c r="K2" t="n">
+        <v>8</v>
+      </c>
+      <c r="L2" t="n">
+        <v>9</v>
+      </c>
+      <c r="M2" t="n">
+        <v>4</v>
+      </c>
+      <c r="N2" t="n">
+        <v>5</v>
+      </c>
+      <c r="O2" t="n">
+        <v>6</v>
+      </c>
+      <c r="P2" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>6</v>
+      </c>
+      <c r="R2" t="n">
+        <v>4</v>
+      </c>
+      <c r="S2" t="n">
+        <v>7</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>4</v>
+      </c>
+      <c r="V2" t="n">
+        <v>7</v>
+      </c>
+      <c r="W2" t="n">
+        <v>7</v>
+      </c>
+      <c r="X2" t="n">
+        <v>9</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>6</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>7</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -494,19 +716,103 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="n">
         <v>7</v>
       </c>
       <c r="D3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>8</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>7</v>
+      </c>
+      <c r="J3" t="n">
+        <v>3</v>
+      </c>
+      <c r="K3" t="n">
+        <v>10</v>
+      </c>
+      <c r="L3" t="n">
+        <v>8</v>
+      </c>
+      <c r="M3" t="n">
+        <v>4</v>
+      </c>
+      <c r="N3" t="n">
+        <v>7</v>
+      </c>
+      <c r="O3" t="n">
+        <v>7</v>
+      </c>
+      <c r="P3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>7</v>
+      </c>
+      <c r="R3" t="n">
+        <v>7</v>
+      </c>
+      <c r="S3" t="n">
+        <v>3</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>6</v>
+      </c>
+      <c r="V3" t="n">
+        <v>6</v>
+      </c>
+      <c r="W3" t="n">
+        <v>3</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -519,15 +825,99 @@
         <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>5</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N4" t="n">
+        <v>3</v>
+      </c>
+      <c r="O4" t="n">
+        <v>3</v>
+      </c>
+      <c r="P4" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>2</v>
+      </c>
+      <c r="R4" t="n">
+        <v>7</v>
+      </c>
+      <c r="S4" t="n">
+        <v>6</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>7</v>
+      </c>
+      <c r="V4" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" t="n">
+        <v>4</v>
+      </c>
+      <c r="X4" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>9</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>9</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH4" t="n">
         <v>5</v>
       </c>
     </row>
@@ -538,19 +928,93 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>7</v>
+      </c>
+      <c r="M5" t="n">
+        <v>3</v>
+      </c>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="n">
+        <v>9</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>6</v>
+      </c>
+      <c r="R5" t="n">
+        <v>10</v>
+      </c>
+      <c r="S5" t="n">
+        <v>10</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>10</v>
+      </c>
+      <c r="V5" t="n">
+        <v>4</v>
+      </c>
+      <c r="W5" t="n">
+        <v>10</v>
+      </c>
+      <c r="X5" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -560,19 +1024,103 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>6</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>4</v>
+      </c>
+      <c r="L6" t="n">
+        <v>3</v>
+      </c>
+      <c r="M6" t="n">
+        <v>6</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" t="n">
+        <v>8</v>
+      </c>
+      <c r="P6" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>3</v>
+      </c>
+      <c r="R6" t="n">
+        <v>7</v>
+      </c>
+      <c r="S6" t="n">
+        <v>6</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>1</v>
+      </c>
+      <c r="V6" t="n">
+        <v>4</v>
+      </c>
+      <c r="W6" t="n">
+        <v>7</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>7</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>9</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>6</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -582,19 +1130,101 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" t="n">
         <v>8</v>
       </c>
       <c r="D7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>10</v>
+      </c>
+      <c r="I7" t="n">
+        <v>9</v>
+      </c>
+      <c r="J7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" t="n">
+        <v>9</v>
+      </c>
+      <c r="L7" t="n">
+        <v>10</v>
+      </c>
+      <c r="M7" t="n">
+        <v>8</v>
+      </c>
+      <c r="N7" t="n">
+        <v>10</v>
+      </c>
+      <c r="O7" t="n">
+        <v>6</v>
+      </c>
+      <c r="P7" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>7</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" t="n">
+        <v>10</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>2</v>
+      </c>
+      <c r="V7" t="n">
+        <v>5</v>
+      </c>
+      <c r="W7" t="n">
+        <v>7</v>
+      </c>
+      <c r="X7" t="n">
+        <v>9</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>9</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>6</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -604,19 +1234,101 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>9</v>
+      </c>
+      <c r="I8" t="n">
+        <v>7</v>
+      </c>
+      <c r="J8" t="n">
+        <v>9</v>
+      </c>
+      <c r="K8" t="n">
+        <v>9</v>
+      </c>
+      <c r="L8" t="n">
+        <v>10</v>
+      </c>
+      <c r="M8" t="n">
+        <v>4</v>
+      </c>
+      <c r="N8" t="n">
+        <v>7</v>
+      </c>
+      <c r="O8" t="n">
+        <v>6</v>
+      </c>
+      <c r="P8" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>9</v>
+      </c>
+      <c r="R8" t="n">
+        <v>2</v>
+      </c>
+      <c r="S8" t="n">
+        <v>9</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>4</v>
+      </c>
+      <c r="V8" t="n">
+        <v>5</v>
+      </c>
+      <c r="W8" t="n">
+        <v>8</v>
+      </c>
+      <c r="X8" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>10</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -626,19 +1338,101 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>4</v>
+      </c>
+      <c r="I9" t="n">
+        <v>10</v>
+      </c>
+      <c r="J9" t="n">
+        <v>8</v>
+      </c>
+      <c r="K9" t="n">
+        <v>7</v>
+      </c>
+      <c r="L9" t="n">
+        <v>5</v>
+      </c>
+      <c r="M9" t="n">
+        <v>3</v>
+      </c>
+      <c r="N9" t="n">
+        <v>3</v>
+      </c>
+      <c r="O9" t="n">
+        <v>6</v>
+      </c>
+      <c r="P9" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>4</v>
+      </c>
+      <c r="R9" t="n">
+        <v>8</v>
+      </c>
+      <c r="S9" t="n">
+        <v>2</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>9</v>
+      </c>
+      <c r="V9" t="n">
+        <v>10</v>
+      </c>
+      <c r="W9" t="n">
+        <v>2</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>7</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -648,19 +1442,103 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D10" t="n">
         <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>4</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>10</v>
+      </c>
+      <c r="K10" t="n">
+        <v>5</v>
+      </c>
+      <c r="L10" t="n">
+        <v>4</v>
+      </c>
+      <c r="M10" t="n">
+        <v>8</v>
+      </c>
+      <c r="N10" t="n">
+        <v>7</v>
+      </c>
+      <c r="O10" t="n">
+        <v>8</v>
+      </c>
+      <c r="P10" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>10</v>
+      </c>
+      <c r="R10" t="n">
+        <v>2</v>
+      </c>
+      <c r="S10" t="n">
+        <v>8</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>3</v>
+      </c>
+      <c r="V10" t="n">
+        <v>4</v>
+      </c>
+      <c r="W10" t="n">
+        <v>7</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>7</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>7</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>8</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>7</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -673,16 +1551,100 @@
         <v>4</v>
       </c>
       <c r="C11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" t="n">
+        <v>7</v>
+      </c>
+      <c r="J11" t="n">
+        <v>10</v>
+      </c>
+      <c r="K11" t="n">
+        <v>10</v>
+      </c>
+      <c r="L11" t="n">
+        <v>9</v>
+      </c>
+      <c r="M11" t="n">
+        <v>6</v>
+      </c>
+      <c r="N11" t="n">
+        <v>6</v>
+      </c>
+      <c r="O11" t="n">
+        <v>9</v>
+      </c>
+      <c r="P11" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>10</v>
+      </c>
+      <c r="R11" t="n">
+        <v>2</v>
+      </c>
+      <c r="S11" t="n">
+        <v>7</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>6</v>
+      </c>
+      <c r="V11" t="n">
+        <v>7</v>
+      </c>
+      <c r="W11" t="n">
+        <v>4</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>7</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>7</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>8</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="12">
@@ -692,19 +1654,103 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D12" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" t="n">
         <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>6</v>
+      </c>
+      <c r="I12" t="n">
+        <v>10</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" t="n">
+        <v>8</v>
+      </c>
+      <c r="L12" t="n">
+        <v>7</v>
+      </c>
+      <c r="M12" t="n">
+        <v>2</v>
+      </c>
+      <c r="N12" t="n">
+        <v>10</v>
+      </c>
+      <c r="O12" t="n">
+        <v>8</v>
+      </c>
+      <c r="P12" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>8</v>
+      </c>
+      <c r="R12" t="n">
+        <v>4</v>
+      </c>
+      <c r="S12" t="n">
+        <v>5</v>
+      </c>
+      <c r="T12" t="n">
+        <v>10</v>
+      </c>
+      <c r="U12" t="n">
+        <v>8</v>
+      </c>
+      <c r="V12" t="n">
+        <v>10</v>
+      </c>
+      <c r="W12" t="n">
+        <v>3</v>
+      </c>
+      <c r="X12" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>8</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -717,16 +1763,98 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>8</v>
+      </c>
+      <c r="I13" t="n">
+        <v>10</v>
+      </c>
+      <c r="J13" t="n">
+        <v>9</v>
+      </c>
+      <c r="K13" t="n">
+        <v>6</v>
+      </c>
+      <c r="L13" t="n">
+        <v>2</v>
+      </c>
+      <c r="M13" t="n">
+        <v>7</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>6</v>
+      </c>
+      <c r="P13" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>5</v>
+      </c>
+      <c r="R13" t="n">
+        <v>7</v>
+      </c>
+      <c r="S13" t="n">
+        <v>1</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>9</v>
+      </c>
+      <c r="V13" t="n">
+        <v>7</v>
+      </c>
+      <c r="W13" t="n">
+        <v>5</v>
+      </c>
+      <c r="X13" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="14">
@@ -736,19 +1864,101 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" t="n">
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>3</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>10</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>5</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" t="n">
+        <v>2</v>
+      </c>
+      <c r="M14" t="n">
+        <v>9</v>
+      </c>
+      <c r="N14" t="n">
+        <v>9</v>
+      </c>
+      <c r="O14" t="n">
+        <v>2</v>
+      </c>
+      <c r="P14" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>5</v>
+      </c>
+      <c r="R14" t="n">
+        <v>10</v>
+      </c>
+      <c r="S14" t="n">
+        <v>1</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>8</v>
+      </c>
+      <c r="V14" t="n">
+        <v>3</v>
+      </c>
+      <c r="W14" t="n">
+        <v>6</v>
+      </c>
+      <c r="X14" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>8</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="15">
@@ -758,19 +1968,103 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E15" t="n">
         <v>7</v>
       </c>
       <c r="F15" t="n">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>10</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>10</v>
+      </c>
+      <c r="K15" t="n">
+        <v>6</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" t="n">
+        <v>9</v>
+      </c>
+      <c r="N15" t="n">
+        <v>4</v>
+      </c>
+      <c r="O15" t="n">
+        <v>6</v>
+      </c>
+      <c r="P15" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>7</v>
+      </c>
+      <c r="S15" t="n">
+        <v>5</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>7</v>
+      </c>
+      <c r="V15" t="n">
+        <v>2</v>
+      </c>
+      <c r="W15" t="n">
+        <v>10</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>6</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>7</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -780,19 +2074,103 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C16" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D16" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>9</v>
+      </c>
+      <c r="J16" t="n">
+        <v>5</v>
+      </c>
+      <c r="K16" t="n">
+        <v>2</v>
+      </c>
+      <c r="L16" t="n">
+        <v>7</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>3</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>9</v>
+      </c>
+      <c r="R16" t="n">
+        <v>10</v>
+      </c>
+      <c r="S16" t="n">
+        <v>4</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>9</v>
+      </c>
+      <c r="V16" t="n">
+        <v>8</v>
+      </c>
+      <c r="W16" t="n">
+        <v>4</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>10</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>9</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="17">
@@ -802,19 +2180,101 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C17" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D17" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>9</v>
+      </c>
+      <c r="I17" t="n">
+        <v>9</v>
+      </c>
+      <c r="J17" t="n">
+        <v>7</v>
+      </c>
+      <c r="K17" t="n">
+        <v>7</v>
+      </c>
+      <c r="L17" t="n">
+        <v>6</v>
+      </c>
+      <c r="M17" t="n">
+        <v>6</v>
+      </c>
+      <c r="N17" t="n">
+        <v>2</v>
+      </c>
+      <c r="O17" t="n">
+        <v>2</v>
+      </c>
+      <c r="P17" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>2</v>
+      </c>
+      <c r="R17" t="n">
+        <v>7</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>10</v>
+      </c>
+      <c r="V17" t="n">
+        <v>10</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG17" t="inlineStr"/>
+      <c r="AH17" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -824,19 +2284,103 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>7</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>3</v>
+      </c>
+      <c r="K18" t="n">
+        <v>3</v>
+      </c>
+      <c r="L18" t="n">
+        <v>4</v>
+      </c>
+      <c r="M18" t="n">
+        <v>10</v>
+      </c>
+      <c r="N18" t="n">
+        <v>5</v>
+      </c>
+      <c r="O18" t="n">
+        <v>10</v>
+      </c>
+      <c r="P18" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>10</v>
+      </c>
+      <c r="R18" t="n">
+        <v>2</v>
+      </c>
+      <c r="S18" t="n">
+        <v>9</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" t="n">
+        <v>7</v>
+      </c>
+      <c r="V18" t="n">
+        <v>2</v>
+      </c>
+      <c r="W18" t="n">
+        <v>10</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="19">
@@ -846,19 +2390,101 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D19" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>5</v>
+      </c>
+      <c r="K19" t="n">
+        <v>7</v>
+      </c>
+      <c r="L19" t="n">
+        <v>8</v>
+      </c>
+      <c r="M19" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" t="n">
+        <v>9</v>
+      </c>
+      <c r="O19" t="n">
+        <v>10</v>
+      </c>
+      <c r="P19" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>8</v>
+      </c>
+      <c r="R19" t="n">
+        <v>7</v>
+      </c>
+      <c r="S19" t="n">
+        <v>4</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>3</v>
+      </c>
+      <c r="V19" t="n">
+        <v>9</v>
+      </c>
+      <c r="W19" t="n">
+        <v>2</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG19" t="inlineStr"/>
+      <c r="AH19" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -868,19 +2494,89 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="n">
         <v>3</v>
       </c>
       <c r="D20" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="n">
+        <v>8</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="n">
+        <v>3</v>
+      </c>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="n">
+        <v>10</v>
+      </c>
+      <c r="N20" t="n">
+        <v>5</v>
+      </c>
+      <c r="O20" t="n">
+        <v>10</v>
+      </c>
+      <c r="P20" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>7</v>
+      </c>
+      <c r="R20" t="n">
+        <v>4</v>
+      </c>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="n">
+        <v>1</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" t="n">
+        <v>10</v>
+      </c>
+      <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF20" t="inlineStr"/>
+      <c r="AG20" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="21">
@@ -890,19 +2586,103 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D21" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>9</v>
+      </c>
+      <c r="K21" t="n">
+        <v>4</v>
+      </c>
+      <c r="L21" t="n">
+        <v>5</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" t="n">
+        <v>9</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>4</v>
+      </c>
+      <c r="R21" t="n">
+        <v>8</v>
+      </c>
+      <c r="S21" t="n">
+        <v>3</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" t="n">
+        <v>5</v>
+      </c>
+      <c r="V21" t="n">
+        <v>9</v>
+      </c>
+      <c r="W21" t="n">
+        <v>8</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>10</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>8</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="22">
@@ -912,19 +2692,103 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C22" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D22" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>9</v>
+      </c>
+      <c r="I22" t="n">
+        <v>6</v>
+      </c>
+      <c r="J22" t="n">
+        <v>8</v>
+      </c>
+      <c r="K22" t="n">
+        <v>9</v>
+      </c>
+      <c r="L22" t="n">
+        <v>8</v>
+      </c>
+      <c r="M22" t="n">
+        <v>2</v>
+      </c>
+      <c r="N22" t="n">
+        <v>8</v>
+      </c>
+      <c r="O22" t="n">
+        <v>4</v>
+      </c>
+      <c r="P22" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>3</v>
+      </c>
+      <c r="R22" t="n">
+        <v>4</v>
+      </c>
+      <c r="S22" t="n">
+        <v>10</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0</v>
+      </c>
+      <c r="V22" t="n">
+        <v>8</v>
+      </c>
+      <c r="W22" t="n">
+        <v>3</v>
+      </c>
+      <c r="X22" t="n">
+        <v>9</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>7</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -934,19 +2798,103 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C23" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D23" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E23" t="n">
         <v>9</v>
       </c>
       <c r="F23" t="n">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>7</v>
+      </c>
+      <c r="I23" t="n">
+        <v>6</v>
+      </c>
+      <c r="J23" t="n">
+        <v>7</v>
+      </c>
+      <c r="K23" t="n">
+        <v>4</v>
+      </c>
+      <c r="L23" t="n">
+        <v>3</v>
+      </c>
+      <c r="M23" t="n">
+        <v>7</v>
+      </c>
+      <c r="N23" t="n">
+        <v>4</v>
+      </c>
+      <c r="O23" t="n">
+        <v>4</v>
+      </c>
+      <c r="P23" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>1</v>
+      </c>
+      <c r="R23" t="n">
+        <v>10</v>
+      </c>
+      <c r="S23" t="n">
+        <v>3</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0</v>
+      </c>
+      <c r="U23" t="n">
+        <v>4</v>
+      </c>
+      <c r="V23" t="n">
+        <v>3</v>
+      </c>
+      <c r="W23" t="n">
+        <v>6</v>
+      </c>
+      <c r="X23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>9</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>9</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>9</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -956,18 +2904,100 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C24" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D24" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E24" t="n">
         <v>6</v>
       </c>
       <c r="F24" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>7</v>
+      </c>
+      <c r="I24" t="n">
+        <v>8</v>
+      </c>
+      <c r="J24" t="n">
+        <v>8</v>
+      </c>
+      <c r="K24" t="n">
+        <v>5</v>
+      </c>
+      <c r="L24" t="n">
+        <v>3</v>
+      </c>
+      <c r="M24" t="n">
+        <v>7</v>
+      </c>
+      <c r="N24" t="n">
+        <v>8</v>
+      </c>
+      <c r="O24" t="n">
+        <v>7</v>
+      </c>
+      <c r="P24" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>4</v>
+      </c>
+      <c r="R24" t="n">
+        <v>8</v>
+      </c>
+      <c r="S24" t="n">
+        <v>9</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U24" t="n">
+        <v>5</v>
+      </c>
+      <c r="V24" t="n">
+        <v>6</v>
+      </c>
+      <c r="W24" t="n">
+        <v>1</v>
+      </c>
+      <c r="X24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>6</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>9</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG24" t="inlineStr"/>
+      <c r="AH24" t="n">
         <v>6</v>
       </c>
     </row>
@@ -978,19 +3008,103 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D25" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>4</v>
+      </c>
+      <c r="I25" t="n">
+        <v>5</v>
+      </c>
+      <c r="J25" t="n">
+        <v>6</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1</v>
+      </c>
+      <c r="M25" t="n">
+        <v>9</v>
+      </c>
+      <c r="N25" t="n">
+        <v>2</v>
+      </c>
+      <c r="O25" t="n">
+        <v>3</v>
+      </c>
+      <c r="P25" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>5</v>
+      </c>
+      <c r="R25" t="n">
+        <v>10</v>
+      </c>
+      <c r="S25" t="n">
+        <v>2</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" t="n">
+        <v>10</v>
+      </c>
+      <c r="V25" t="n">
+        <v>1</v>
+      </c>
+      <c r="W25" t="n">
+        <v>9</v>
+      </c>
+      <c r="X25" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="26">
@@ -1000,10 +3114,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26" t="n">
         <v>5</v>
@@ -1012,7 +3126,91 @@
         <v>4</v>
       </c>
       <c r="F26" t="n">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>3</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>2</v>
+      </c>
+      <c r="K26" t="n">
+        <v>2</v>
+      </c>
+      <c r="L26" t="n">
+        <v>5</v>
+      </c>
+      <c r="M26" t="n">
+        <v>5</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1</v>
+      </c>
+      <c r="O26" t="n">
+        <v>4</v>
+      </c>
+      <c r="P26" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>1</v>
+      </c>
+      <c r="R26" t="n">
+        <v>10</v>
+      </c>
+      <c r="S26" t="n">
+        <v>5</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0</v>
+      </c>
+      <c r="U26" t="n">
+        <v>6</v>
+      </c>
+      <c r="V26" t="n">
+        <v>2</v>
+      </c>
+      <c r="W26" t="n">
+        <v>9</v>
+      </c>
+      <c r="X26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>7</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -1022,19 +3220,103 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C27" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D27" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E27" t="n">
         <v>2</v>
       </c>
       <c r="F27" t="n">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>6</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K27" t="n">
+        <v>6</v>
+      </c>
+      <c r="L27" t="n">
+        <v>6</v>
+      </c>
+      <c r="M27" t="n">
+        <v>5</v>
+      </c>
+      <c r="N27" t="n">
+        <v>6</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1</v>
+      </c>
+      <c r="P27" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>2</v>
+      </c>
+      <c r="R27" t="n">
+        <v>7</v>
+      </c>
+      <c r="S27" t="n">
+        <v>7</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0</v>
+      </c>
+      <c r="U27" t="n">
+        <v>2</v>
+      </c>
+      <c r="V27" t="n">
+        <v>6</v>
+      </c>
+      <c r="W27" t="n">
+        <v>1</v>
+      </c>
+      <c r="X27" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>9</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="28">
@@ -1044,19 +3326,103 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C28" t="n">
         <v>9</v>
       </c>
       <c r="D28" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>2</v>
+      </c>
+      <c r="I28" t="n">
+        <v>8</v>
+      </c>
+      <c r="J28" t="n">
+        <v>7</v>
+      </c>
+      <c r="K28" t="n">
+        <v>10</v>
+      </c>
+      <c r="L28" t="n">
+        <v>10</v>
+      </c>
+      <c r="M28" t="n">
+        <v>2</v>
+      </c>
+      <c r="N28" t="n">
+        <v>10</v>
+      </c>
+      <c r="O28" t="n">
+        <v>9</v>
+      </c>
+      <c r="P28" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>9</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="n">
+        <v>8</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0</v>
+      </c>
+      <c r="U28" t="n">
+        <v>2</v>
+      </c>
+      <c r="V28" t="n">
+        <v>9</v>
+      </c>
+      <c r="W28" t="n">
+        <v>5</v>
+      </c>
+      <c r="X28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>9</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>